<commit_message>
Finally test case runs successfully. New customer added successfully
</commit_message>
<xml_diff>
--- a/InputData/InputData.xlsx
+++ b/InputData/InputData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15300" windowHeight="4470"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15300" windowHeight="2865"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -490,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>